<commit_message>
Pergantian dummy dataset dan update script
</commit_message>
<xml_diff>
--- a/dataset/data_acuan.xlsx
+++ b/dataset/data_acuan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Computer Science\PKL\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Computer Science\PKL\Pemeriksa Ketepatan Waktu Update\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B33AA2-C521-486C-82A1-CBDCF48B9D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC19050-4185-4772-9F2F-824C062A26FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D673CD0-97D5-4D54-9354-D17F6BD8B582}"/>
   </bookViews>
@@ -34,17 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Dashboard</t>
   </si>
   <si>
-    <t>Data_Source</t>
-  </si>
-  <si>
-    <t>Update_by</t>
-  </si>
-  <si>
     <t xml:space="preserve">Update_Periode </t>
   </si>
   <si>
@@ -58,6 +52,15 @@
   </si>
   <si>
     <t>SLA_(Met/Miss)</t>
+  </si>
+  <si>
+    <t>File_Name</t>
+  </si>
+  <si>
+    <t>Source_File</t>
+  </si>
+  <si>
+    <t>Updated_by</t>
   </si>
 </sst>
 </file>
@@ -409,47 +412,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C3CCC4-E55C-4D98-92C9-91767D6BE719}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>